<commit_message>
Version final Anexos #
</commit_message>
<xml_diff>
--- a/src/Avistamientos/GeneracionModelo/resultados.xlsx
+++ b/src/Avistamientos/GeneracionModelo/resultados.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pablo\Documents\GitHub\Jellyfish_Forecast\src\Avistamientos\GeneracionModelo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E1D7782-DE9B-48BC-A8B1-D251063CB319}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B621550E-DFD0-45C9-B7C9-2D812E59B440}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>2__dias__c_celdas_2_splits</t>
   </si>
@@ -40,27 +40,15 @@
     <t>2__dias__c_celdas_10_splits_params</t>
   </si>
   <si>
-    <t>random_forest</t>
-  </si>
-  <si>
-    <t>nearest_neighbor</t>
-  </si>
-  <si>
     <t>SVR</t>
   </si>
   <si>
-    <t>arbol_decision</t>
-  </si>
-  <si>
     <t>MLP</t>
   </si>
   <si>
     <t>Boosting</t>
   </si>
   <si>
-    <t>ensembles</t>
-  </si>
-  <si>
     <t>{'max_depth': None, 'max_features': 'log2', 'n_estimators': 100}</t>
   </si>
   <si>
@@ -113,6 +101,15 @@
   </si>
   <si>
     <t>{'max_depth': 60, 'n_estimators': 359}</t>
+  </si>
+  <si>
+    <t>Random Forest</t>
+  </si>
+  <si>
+    <t>Nearest Neighbor</t>
+  </si>
+  <si>
+    <t>Decission Tree</t>
   </si>
 </sst>
 </file>
@@ -234,16 +231,16 @@
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>random_forest</c:v>
+                  <c:v>Random Forest</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>nearest_neighbor</c:v>
+                  <c:v>Nearest Neighbor</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>SVR</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>arbol_decision</c:v>
+                  <c:v>Decission Tree</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>MLP</c:v>
@@ -514,16 +511,16 @@
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>random_forest</c:v>
+                  <c:v>Random Forest</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>nearest_neighbor</c:v>
+                  <c:v>Nearest Neighbor</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>SVR</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>arbol_decision</c:v>
+                  <c:v>Decission Tree</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>MLP</c:v>
@@ -2217,7 +2214,7 @@
   <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="A2:B7"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2248,146 +2245,144 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>6</v>
+        <v>27</v>
       </c>
       <c r="B2">
         <v>-2.3359899981811309E-2</v>
       </c>
       <c r="C2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D2">
         <v>-0.76615136256749339</v>
       </c>
       <c r="E2" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="F2">
         <v>-1.0220783905856501</v>
       </c>
       <c r="G2" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>7</v>
+        <v>28</v>
       </c>
       <c r="B3">
         <v>1.7389993570974871E-2</v>
       </c>
       <c r="C3" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D3">
         <v>-3.62294231362986</v>
       </c>
       <c r="E3" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="F3">
         <v>-0.40980594602190601</v>
       </c>
       <c r="G3" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B4">
         <v>-3.7600128656750893E-2</v>
       </c>
       <c r="C4" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="D4">
         <v>-6.1785404789621363E-2</v>
       </c>
       <c r="E4" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="F4">
         <v>-0.11801870105662229</v>
       </c>
       <c r="G4" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>9</v>
+        <v>29</v>
       </c>
       <c r="B5">
         <v>0.25236655487189918</v>
       </c>
       <c r="C5" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="D5">
         <v>-0.12798320088042819</v>
       </c>
       <c r="E5" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="F5">
         <v>-0.36381451084646188</v>
       </c>
       <c r="G5" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B6">
         <v>1.6227936353754299E-2</v>
       </c>
       <c r="C6" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D6">
         <v>-9.4521900415365651E-2</v>
       </c>
       <c r="E6" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="F6">
         <v>-0.2046001180273552</v>
       </c>
       <c r="G6" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B7">
         <v>-0.1389970057392734</v>
       </c>
       <c r="C7" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D7">
         <v>-4.8148785166959946</v>
       </c>
       <c r="E7" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="F7">
         <v>-10.21450458732672</v>
       </c>
       <c r="G7" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>12</v>
-      </c>
+      <c r="A8" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>